<commit_message>
Add for Enemy Logic Difficulty and Level Modifier.
I think Enemy is done (logic for enemy is done). Update Excel table with Logic for level modifier.
</commit_message>
<xml_diff>
--- a/RPG/Stats for Console RPG.xlsx
+++ b/RPG/Stats for Console RPG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C++\HOMEWORK C++\RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C84B07-FF92-468B-BE98-6FD26A341433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFC16D5-433A-45F2-A3DA-EC7B537243CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21D6ACE2-8239-4A58-9D1F-7CF56931E1A4}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Hero</t>
   </si>
@@ -54,18 +76,6 @@
     <t>Enemy</t>
   </si>
   <si>
-    <t>Enemy Difficult: Normal</t>
-  </si>
-  <si>
-    <t>Enemy Difficult: Hard</t>
-  </si>
-  <si>
-    <t>Enemy Difficult: Easy</t>
-  </si>
-  <si>
-    <t>Difficult modifier</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -75,7 +85,55 @@
     <t>Hard</t>
   </si>
   <si>
-    <t>Level modifier:</t>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Check Duel</t>
+  </si>
+  <si>
+    <t>Attacks for Kill</t>
+  </si>
+  <si>
+    <t>Time for Kill</t>
+  </si>
+  <si>
+    <t>Result:</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Lose</t>
+  </si>
+  <si>
+    <t>Dealy Attacks</t>
+  </si>
+  <si>
+    <t>Level Enemy Modification</t>
+  </si>
+  <si>
+    <t>Rand Buff</t>
+  </si>
+  <si>
+    <t>Parametrs for duel</t>
+  </si>
+  <si>
+    <t>Hero level</t>
+  </si>
+  <si>
+    <t>Enemy Difficulty: Easy</t>
+  </si>
+  <si>
+    <t>Enemy Difficulty: Normal</t>
+  </si>
+  <si>
+    <t>Enemy Difficulty: Hard</t>
+  </si>
+  <si>
+    <t>Difficulty Enemy modifier</t>
+  </si>
+  <si>
+    <t>Enemy Difficulty</t>
   </si>
 </sst>
 </file>
@@ -129,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -293,25 +351,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -323,9 +368,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,20 +394,32 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -365,6 +436,183 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC0AFC6F-CD51-4A47-A8B1-1D3C1EBC1C94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2057400" y="6334126"/>
+          <a:ext cx="1171575" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Enemy Difficulty:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Easy -	0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Normal</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> -	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Hard -	2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B88C0963-B712-4BA5-A5F8-26DBAE1A3A02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000124" y="5162549"/>
+          <a:ext cx="7743825" cy="3000375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="127000" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>Experimental</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+            <a:t> (work not correctly for now)</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1800" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,18 +914,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831E001F-36F6-465E-AD54-B18F2B607D51}">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="26" max="29" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -702,10 +961,6 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -754,40 +1009,35 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
     </row>
     <row r="3" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="16"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="29"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="29"/>
+      <c r="S3" s="30"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -802,60 +1052,57 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
     </row>
     <row r="4" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="17" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="17" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="17" t="s">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="39" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -866,42 +1113,39 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="20">
+      <c r="C5" s="37">
         <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
       </c>
       <c r="E5" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="9">
-        <v>25</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+        <v>60</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="15"/>
       <c r="I5" s="2">
-        <f>M5*J21</f>
-        <v>90</v>
+        <f>M5+J19</f>
+        <v>85</v>
       </c>
       <c r="J5" s="3">
-        <f>N5*J21</f>
-        <v>4.5</v>
+        <f>N5+K19</f>
+        <v>3.5</v>
       </c>
       <c r="K5" s="9">
-        <f>O5/J21</f>
-        <v>22.222222222222221</v>
-      </c>
-      <c r="L5" s="23"/>
+        <f>O5+L19</f>
+        <v>53</v>
+      </c>
+      <c r="L5" s="15"/>
       <c r="M5" s="2">
         <v>100</v>
       </c>
@@ -909,23 +1153,25 @@
         <v>5</v>
       </c>
       <c r="O5" s="9">
-        <v>20</v>
-      </c>
-      <c r="P5" s="23"/>
+        <v>50</v>
+      </c>
+      <c r="P5" s="15"/>
       <c r="Q5" s="2">
-        <f>M5*J23</f>
-        <v>110.00000000000001</v>
+        <f>M5+J21</f>
+        <v>115</v>
       </c>
       <c r="R5" s="3">
-        <f>N5*J23</f>
-        <v>5.5</v>
+        <f>N5+K21</f>
+        <v>6.5</v>
       </c>
       <c r="S5" s="9">
-        <f>O5/J23</f>
-        <v>18.18181818181818</v>
+        <f>O5+L21</f>
+        <v>47</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -936,73 +1182,69 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="20">
+      <c r="C6" s="37">
         <v>2</v>
       </c>
       <c r="D6" s="4">
-        <f>D5*($F$20*$C$5)</f>
-        <v>105</v>
+        <f ca="1">IF(G6 = 1,D5+$D$19, D5)</f>
+        <v>122</v>
       </c>
       <c r="E6" s="5">
-        <f>E5*($F$20*$C$5)</f>
-        <v>8.4</v>
+        <f ca="1">IF(G6 = 2,E5+E$19, E5)</f>
+        <v>7</v>
       </c>
       <c r="F6" s="6">
-        <f>F5/($F$20*$C$5)</f>
-        <v>23.80952380952381</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+        <f ca="1">IF(G6 = 3,F5-F$19, F5)</f>
+        <v>60</v>
+      </c>
+      <c r="G6" s="40">
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="15"/>
       <c r="I6" s="4">
-        <f>I5*($F$21*$C$5)</f>
-        <v>93.600000000000009</v>
+        <f>I5+O$19</f>
+        <v>90</v>
       </c>
       <c r="J6" s="5">
-        <f>J5*($F$21*$C$5)</f>
-        <v>4.68</v>
+        <f>J5+P$19</f>
+        <v>4</v>
       </c>
       <c r="K6" s="6">
-        <f>K5/($F$21*$C$5)</f>
-        <v>21.367521367521366</v>
-      </c>
-      <c r="L6" s="23"/>
+        <f>K5-Q$19</f>
+        <v>52</v>
+      </c>
+      <c r="L6" s="15"/>
       <c r="M6" s="4">
-        <f>M5*($F$21*$C$5)</f>
-        <v>104</v>
+        <f>M5+O$20</f>
+        <v>105.25</v>
       </c>
       <c r="N6" s="5">
-        <f>N5*($F$21*$C$5)</f>
-        <v>5.2</v>
+        <f>N5+P$20</f>
+        <v>5.75</v>
       </c>
       <c r="O6" s="6">
-        <f>O5/($F$21*$C$5)</f>
-        <v>19.23076923076923</v>
-      </c>
-      <c r="P6" s="23"/>
+        <f>O5-Q$20</f>
+        <v>48</v>
+      </c>
+      <c r="P6" s="15"/>
       <c r="Q6" s="4">
-        <f>Q5*($F$21*$C$5)</f>
-        <v>114.40000000000002</v>
+        <f>Q5+O$21</f>
+        <v>120.5</v>
       </c>
       <c r="R6" s="5">
-        <f>R5*($F$21*$C$5)</f>
-        <v>5.7200000000000006</v>
+        <f>R5+P$21</f>
+        <v>7.5</v>
       </c>
       <c r="S6" s="6">
-        <f>S5/($F$21*$C$5)</f>
-        <v>17.48251748251748</v>
+        <f>S5-Q$21</f>
+        <v>44</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
@@ -1012,73 +1254,69 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="20">
+      <c r="C7" s="37">
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D14" si="0">D6*($F$20*$C$5)</f>
-        <v>110.25</v>
+        <f ca="1">IF(G7 = 1,D6+$D$19, D6)</f>
+        <v>144</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" ref="E7:E14" si="1">E6*($F$20*$C$5)</f>
-        <v>8.82</v>
+        <f ca="1">IF(G7 = 2,E6+E$19, E6)</f>
+        <v>7</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" ref="F7:F14" si="2">F6/($F$20*$C$5)</f>
-        <v>22.675736961451246</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+        <f ca="1">IF(G7 = 3,F6-F$19, F6)</f>
+        <v>60</v>
+      </c>
+      <c r="G7" s="40">
+        <f t="shared" ref="G7:G14" ca="1" si="0">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="15"/>
       <c r="I7" s="4">
-        <f t="shared" ref="I7:I14" si="3">I6*($F$21*$C$5)</f>
-        <v>97.344000000000008</v>
+        <f>I6+O$19</f>
+        <v>95</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" ref="J7:J14" si="4">J6*($F$21*$C$5)</f>
-        <v>4.8671999999999995</v>
+        <f>J6+P$19</f>
+        <v>4.5</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" ref="K7:K14" si="5">K6/($F$21*$C$5)</f>
-        <v>20.545693622616696</v>
-      </c>
-      <c r="L7" s="23"/>
+        <f>K6-Q$19</f>
+        <v>51</v>
+      </c>
+      <c r="L7" s="15"/>
       <c r="M7" s="4">
-        <f t="shared" ref="M7:M14" si="6">M6*($F$21*$C$5)</f>
-        <v>108.16</v>
+        <f>M6+O$20</f>
+        <v>110.5</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" ref="N7:N14" si="7">N6*($F$21*$C$5)</f>
-        <v>5.4080000000000004</v>
+        <f>N6+P$20</f>
+        <v>6.5</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" ref="O7:O14" si="8">O6/($F$21*$C$5)</f>
-        <v>18.491124260355029</v>
-      </c>
-      <c r="P7" s="23"/>
+        <f>O6-Q$20</f>
+        <v>46</v>
+      </c>
+      <c r="P7" s="15"/>
       <c r="Q7" s="4">
-        <f t="shared" ref="Q7:Q14" si="9">Q6*($F$21*$C$5)</f>
-        <v>118.97600000000003</v>
+        <f>Q6+O$21</f>
+        <v>126</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" ref="R7:R14" si="10">R6*($F$21*$C$5)</f>
-        <v>5.9488000000000012</v>
+        <f>R6+P$21</f>
+        <v>8.5</v>
       </c>
       <c r="S7" s="6">
-        <f t="shared" ref="S7:S14" si="11">S6/($F$21*$C$5)</f>
-        <v>16.810112963959114</v>
+        <f>S6-Q$21</f>
+        <v>41</v>
       </c>
       <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -1088,75 +1326,69 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="20">
+      <c r="C8" s="37">
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>115.7625</v>
+        <f ca="1">IF(G8 = 1,D7+$D$19, D7)</f>
+        <v>144</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>9.261000000000001</v>
+        <f ca="1">IF(G8 = 2,E7+E$19, E7)</f>
+        <v>10</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="2"/>
-        <v>21.595939963286899</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+        <f ca="1">IF(G8 = 3,F7-F$19, F7)</f>
+        <v>60</v>
+      </c>
+      <c r="G8" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="15"/>
       <c r="I8" s="4">
-        <f t="shared" si="3"/>
-        <v>101.23776000000001</v>
+        <f>I7+O$19</f>
+        <v>100</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="4"/>
-        <v>5.0618879999999997</v>
+        <f>J7+P$19</f>
+        <v>5</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="5"/>
-        <v>19.755474637131439</v>
-      </c>
-      <c r="L8" s="23"/>
+        <f>K7-Q$19</f>
+        <v>50</v>
+      </c>
+      <c r="L8" s="15"/>
       <c r="M8" s="4">
-        <f t="shared" si="6"/>
-        <v>112.4864</v>
+        <f>M7+O$20</f>
+        <v>115.75</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" si="7"/>
-        <v>5.6243200000000009</v>
+        <f>N7+P$20</f>
+        <v>7.25</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="8"/>
-        <v>17.779927173418297</v>
-      </c>
-      <c r="P8" s="23"/>
+        <f>O7-Q$20</f>
+        <v>44</v>
+      </c>
+      <c r="P8" s="15"/>
       <c r="Q8" s="4">
-        <f t="shared" si="9"/>
-        <v>123.73504000000003</v>
+        <f>Q7+O$21</f>
+        <v>131.5</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="10"/>
-        <v>6.1867520000000011</v>
+        <f>R7+P$21</f>
+        <v>9.5</v>
       </c>
       <c r="S8" s="6">
-        <f t="shared" si="11"/>
-        <v>16.163570157652995</v>
+        <f>S7-Q$21</f>
+        <v>38</v>
       </c>
       <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
@@ -1166,75 +1398,69 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="20">
+      <c r="C9" s="37">
         <v>5</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>121.55062500000001</v>
+        <f ca="1">IF(G9 = 1,D8+$D$19, D8)</f>
+        <v>144</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>9.7240500000000019</v>
+        <f ca="1">IF(G9 = 2,E8+E$19, E8)</f>
+        <v>10</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="2"/>
-        <v>20.567561869797046</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+        <f ca="1">IF(G9 = 3,F8-F$19, F8)</f>
+        <v>56</v>
+      </c>
+      <c r="G9" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="15"/>
       <c r="I9" s="4">
-        <f t="shared" si="3"/>
-        <v>105.28727040000001</v>
+        <f>I8+O$19</f>
+        <v>105</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="4"/>
-        <v>5.2643635199999999</v>
+        <f>J8+P$19</f>
+        <v>5.5</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="5"/>
-        <v>18.995648689549459</v>
-      </c>
-      <c r="L9" s="23"/>
+        <f>K8-Q$19</f>
+        <v>49</v>
+      </c>
+      <c r="L9" s="15"/>
       <c r="M9" s="4">
-        <f t="shared" si="6"/>
-        <v>116.98585600000001</v>
+        <f>M8+O$20</f>
+        <v>121</v>
       </c>
       <c r="N9" s="5">
-        <f t="shared" si="7"/>
-        <v>5.8492928000000015</v>
+        <f>N8+P$20</f>
+        <v>8</v>
       </c>
       <c r="O9" s="6">
-        <f t="shared" si="8"/>
-        <v>17.096083820594515</v>
-      </c>
-      <c r="P9" s="23"/>
+        <f>O8-Q$20</f>
+        <v>42</v>
+      </c>
+      <c r="P9" s="15"/>
       <c r="Q9" s="4">
-        <f t="shared" si="9"/>
-        <v>128.68444160000004</v>
+        <f>Q8+O$21</f>
+        <v>137</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="10"/>
-        <v>6.4342220800000014</v>
+        <f>R8+P$21</f>
+        <v>10.5</v>
       </c>
       <c r="S9" s="6">
-        <f t="shared" si="11"/>
-        <v>15.541894382358649</v>
+        <f>S8-Q$21</f>
+        <v>35</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1244,75 +1470,69 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="20">
+      <c r="C10" s="37">
         <v>6</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>127.62815625000002</v>
+        <f ca="1">IF(G10 = 1,D9+$D$19, D9)</f>
+        <v>144</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>10.210252500000003</v>
+        <f ca="1">IF(G10 = 2,E9+E$19, E9)</f>
+        <v>13</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="2"/>
-        <v>19.588154161711472</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+        <f ca="1">IF(G10 = 3,F9-F$19, F9)</f>
+        <v>56</v>
+      </c>
+      <c r="G10" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="15"/>
       <c r="I10" s="4">
-        <f t="shared" si="3"/>
-        <v>109.49876121600002</v>
+        <f>I9+O$19</f>
+        <v>110</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="4"/>
-        <v>5.4749380608000005</v>
+        <f>J9+P$19</f>
+        <v>6</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="5"/>
-        <v>18.265046816874477</v>
-      </c>
-      <c r="L10" s="23"/>
+        <f>K9-Q$19</f>
+        <v>48</v>
+      </c>
+      <c r="L10" s="15"/>
       <c r="M10" s="4">
-        <f t="shared" si="6"/>
-        <v>121.66529024000002</v>
+        <f>M9+O$20</f>
+        <v>126.25</v>
       </c>
       <c r="N10" s="5">
-        <f t="shared" si="7"/>
-        <v>6.0832645120000022</v>
+        <f>N9+P$20</f>
+        <v>8.75</v>
       </c>
       <c r="O10" s="6">
-        <f t="shared" si="8"/>
-        <v>16.438542135187035</v>
-      </c>
-      <c r="P10" s="23"/>
+        <f>O9-Q$20</f>
+        <v>40</v>
+      </c>
+      <c r="P10" s="15"/>
       <c r="Q10" s="4">
-        <f t="shared" si="9"/>
-        <v>133.83181926400005</v>
+        <f>Q9+O$21</f>
+        <v>142.5</v>
       </c>
       <c r="R10" s="5">
-        <f t="shared" si="10"/>
-        <v>6.6915909632000012</v>
+        <f>R9+P$21</f>
+        <v>11.5</v>
       </c>
       <c r="S10" s="6">
-        <f t="shared" si="11"/>
-        <v>14.944129213806393</v>
+        <f>S9-Q$21</f>
+        <v>32</v>
       </c>
       <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -1322,75 +1542,69 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="20">
+      <c r="C11" s="37">
         <v>7</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>134.00956406250003</v>
+        <f ca="1">IF(G11 = 1,D10+$D$19, D10)</f>
+        <v>166</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>10.720765125000003</v>
+        <f ca="1">IF(G11 = 2,E10+E$19, E10)</f>
+        <v>13</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="2"/>
-        <v>18.655384915915686</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+        <f ca="1">IF(G11 = 3,F10-F$19, F10)</f>
+        <v>56</v>
+      </c>
+      <c r="G11" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="15"/>
       <c r="I11" s="4">
-        <f t="shared" si="3"/>
-        <v>113.87871166464002</v>
+        <f>I10+O$19</f>
+        <v>115</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="4"/>
-        <v>5.6939355832320002</v>
+        <f>J10+P$19</f>
+        <v>6.5</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="5"/>
-        <v>17.562545016225457</v>
-      </c>
-      <c r="L11" s="23"/>
+        <f>K10-Q$19</f>
+        <v>47</v>
+      </c>
+      <c r="L11" s="15"/>
       <c r="M11" s="4">
-        <f t="shared" si="6"/>
-        <v>126.53190184960002</v>
+        <f>M10+O$20</f>
+        <v>131.5</v>
       </c>
       <c r="N11" s="5">
-        <f t="shared" si="7"/>
-        <v>6.3265950924800025</v>
+        <f>N10+P$20</f>
+        <v>9.5</v>
       </c>
       <c r="O11" s="6">
-        <f t="shared" si="8"/>
-        <v>15.806290514602917</v>
-      </c>
-      <c r="P11" s="23"/>
+        <f>O10-Q$20</f>
+        <v>38</v>
+      </c>
+      <c r="P11" s="15"/>
       <c r="Q11" s="4">
-        <f t="shared" si="9"/>
-        <v>139.18509203456006</v>
+        <f>Q10+O$21</f>
+        <v>148</v>
       </c>
       <c r="R11" s="5">
-        <f t="shared" si="10"/>
-        <v>6.9592546017280013</v>
+        <f>R10+P$21</f>
+        <v>12.5</v>
       </c>
       <c r="S11" s="6">
-        <f t="shared" si="11"/>
-        <v>14.369355013275378</v>
+        <f>S10-Q$21</f>
+        <v>29</v>
       </c>
       <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -1400,75 +1614,69 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="20">
+      <c r="C12" s="37">
         <v>8</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="0"/>
-        <v>140.71004226562505</v>
+        <f ca="1">IF(G12 = 1,D11+$D$19, D11)</f>
+        <v>166</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>11.256803381250004</v>
+        <f ca="1">IF(G12 = 2,E11+E$19, E11)</f>
+        <v>16</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="2"/>
-        <v>17.767033253253032</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+        <f ca="1">IF(G12 = 3,F11-F$19, F11)</f>
+        <v>56</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="15"/>
       <c r="I12" s="4">
-        <f t="shared" si="3"/>
-        <v>118.43386013122563</v>
+        <f>I11+O$19</f>
+        <v>120</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="4"/>
-        <v>5.9216930065612807</v>
+        <f>J11+P$19</f>
+        <v>7</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="5"/>
-        <v>16.8870625156014</v>
-      </c>
-      <c r="L12" s="23"/>
+        <f>K11-Q$19</f>
+        <v>46</v>
+      </c>
+      <c r="L12" s="15"/>
       <c r="M12" s="4">
-        <f t="shared" si="6"/>
-        <v>131.59317792358402</v>
+        <f>M11+O$20</f>
+        <v>136.75</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" si="7"/>
-        <v>6.5796588961792031</v>
+        <f>N11+P$20</f>
+        <v>10.25</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="8"/>
-        <v>15.198356264041266</v>
-      </c>
-      <c r="P12" s="23"/>
+        <f>O11-Q$20</f>
+        <v>36</v>
+      </c>
+      <c r="P12" s="15"/>
       <c r="Q12" s="4">
-        <f t="shared" si="9"/>
-        <v>144.75249571594247</v>
+        <f>Q11+O$21</f>
+        <v>153.5</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="10"/>
-        <v>7.2376247857971219</v>
+        <f>R11+P$21</f>
+        <v>13.5</v>
       </c>
       <c r="S12" s="6">
-        <f t="shared" si="11"/>
-        <v>13.816687512764785</v>
+        <f>S11-Q$21</f>
+        <v>26</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -1478,69 +1686,67 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="20">
+      <c r="C13" s="37">
         <v>9</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="0"/>
-        <v>147.74554437890632</v>
+        <f ca="1">IF(G13 = 1,D12+$D$19, D12)</f>
+        <v>188</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>11.819643550312504</v>
+        <f ca="1">IF(G13 = 2,E12+E$19, E12)</f>
+        <v>16</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="2"/>
-        <v>16.920984050717173</v>
-      </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+        <f ca="1">IF(G13 = 3,F12-F$19, F12)</f>
+        <v>56</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H13" s="15"/>
       <c r="I13" s="4">
-        <f t="shared" si="3"/>
-        <v>123.17121453647466</v>
+        <f>I12+O$19</f>
+        <v>125</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="4"/>
-        <v>6.1585607268237323</v>
+        <f>J12+P$19</f>
+        <v>7.5</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="5"/>
-        <v>16.23756011115519</v>
-      </c>
-      <c r="L13" s="23"/>
+        <f>K12-Q$19</f>
+        <v>45</v>
+      </c>
+      <c r="L13" s="15"/>
       <c r="M13" s="4">
-        <f t="shared" si="6"/>
-        <v>136.85690504052738</v>
+        <f>M12+O$20</f>
+        <v>142</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" si="7"/>
-        <v>6.8428452520263718</v>
+        <f>N12+P$20</f>
+        <v>11</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="8"/>
-        <v>14.613804100039678</v>
-      </c>
-      <c r="P13" s="23"/>
+        <f>O12-Q$20</f>
+        <v>34</v>
+      </c>
+      <c r="P13" s="15"/>
       <c r="Q13" s="4">
-        <f t="shared" si="9"/>
-        <v>150.54259554458017</v>
+        <f>Q12+O$21</f>
+        <v>159</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" si="10"/>
-        <v>7.5271297772290069</v>
+        <f>R12+P$21</f>
+        <v>14.5</v>
       </c>
       <c r="S13" s="6">
-        <f t="shared" si="11"/>
-        <v>13.285276454581524</v>
+        <f>S12-Q$21</f>
+        <v>23</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
@@ -1556,69 +1762,67 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
     </row>
     <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="21">
+      <c r="C14" s="38">
         <v>10</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" si="0"/>
-        <v>155.13282159785163</v>
+        <f ca="1">IF(G14 = 1,D13+$D$19, D13)</f>
+        <v>188</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="1"/>
-        <v>12.41062572782813</v>
+        <f ca="1">IF(G14 = 2,E13+E$19, E13)</f>
+        <v>19</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="2"/>
-        <v>16.115222905444927</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+        <f ca="1">IF(G14 = 3,F13-F$19, F13)</f>
+        <v>56</v>
+      </c>
+      <c r="G14" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="16"/>
       <c r="I14" s="10">
-        <f t="shared" si="3"/>
-        <v>128.09806311793366</v>
+        <f>I13+O$19</f>
+        <v>130</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="4"/>
-        <v>6.4049031558966822</v>
+        <f>J13+P$19</f>
+        <v>8</v>
       </c>
       <c r="K14" s="8">
-        <f t="shared" si="5"/>
-        <v>15.613038568418451</v>
-      </c>
-      <c r="L14" s="24"/>
+        <f>K13-Q$19</f>
+        <v>44</v>
+      </c>
+      <c r="L14" s="16"/>
       <c r="M14" s="10">
-        <f t="shared" si="6"/>
-        <v>142.33118124214849</v>
+        <f>M13+O$20</f>
+        <v>147.25</v>
       </c>
       <c r="N14" s="7">
-        <f t="shared" si="7"/>
-        <v>7.1165590621074273</v>
+        <f>N13+P$20</f>
+        <v>11.75</v>
       </c>
       <c r="O14" s="8">
-        <f t="shared" si="8"/>
-        <v>14.051734711576612</v>
-      </c>
-      <c r="P14" s="24"/>
+        <f>O13-Q$20</f>
+        <v>32</v>
+      </c>
+      <c r="P14" s="16"/>
       <c r="Q14" s="10">
-        <f t="shared" si="9"/>
-        <v>156.56429936636337</v>
+        <f>Q13+O$21</f>
+        <v>164.5</v>
       </c>
       <c r="R14" s="7">
-        <f t="shared" si="10"/>
-        <v>7.8282149683181679</v>
+        <f>R13+P$21</f>
+        <v>15.5</v>
       </c>
       <c r="S14" s="8">
-        <f t="shared" si="11"/>
-        <v>12.774304283251466</v>
+        <f>S13-Q$21</f>
+        <v>20</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -1634,11 +1838,6 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
-      <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
-      <c r="AL14" s="1"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1674,13 +1873,8 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
-      <c r="AL15" s="1"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1720,24 +1914,30 @@
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="30"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="N17" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="30"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1760,24 +1960,42 @@
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1803,21 +2021,45 @@
     <row r="19" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <v>22</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3</v>
+      </c>
+      <c r="F19" s="8">
+        <v>4</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="I19" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="5">
+        <v>-15</v>
+      </c>
+      <c r="K19" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="L19" s="6">
+        <v>3</v>
+      </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="N19" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="2">
+        <v>5</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>1</v>
+      </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -1840,32 +2082,43 @@
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
     </row>
-    <row r="20" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>1.05</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="I20" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="5">
+        <f>J19-$J$19</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <f>K19-$K$19</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
+        <f>L19-$L$19</f>
+        <v>0</v>
+      </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="N20" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="4">
+        <v>5.25</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>2</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -1891,29 +2144,40 @@
     <row r="21" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="12">
-        <v>1.04</v>
-      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="I21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="7">
+        <f>J20-$J$19</f>
+        <v>15</v>
+      </c>
+      <c r="K21" s="7">
+        <f>K20-$K$19</f>
+        <v>1.5</v>
+      </c>
+      <c r="L21" s="8">
+        <f>L20-$L$19</f>
+        <v>-3</v>
+      </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="N21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O21" s="42">
+        <v>5.5</v>
+      </c>
+      <c r="P21" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>3</v>
+      </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -1939,25 +2203,6 @@
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="6">
-        <v>1</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -1980,28 +2225,10 @@
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
     </row>
-    <row r="23" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="13">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="52"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -2027,21 +2254,6 @@
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -2224,7 +2436,7 @@
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2264,17 +2476,19 @@
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="C30" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="44"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2304,17 +2518,25 @@
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="C31" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2344,17 +2566,30 @@
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="C32" s="31">
+        <v>1</v>
+      </c>
+      <c r="D32" s="11">
+        <v>2</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="47" cm="1">
+        <f t="array" aca="1" ref="H32" ca="1">INDIRECT(ADDRESS(4+$C$32,4))</f>
+        <v>100</v>
+      </c>
+      <c r="I32" s="47" cm="1">
+        <f t="array" aca="1" ref="I32" ca="1">INDIRECT(ADDRESS(4+$C$32,5))</f>
+        <v>7</v>
+      </c>
+      <c r="J32" s="49" cm="1">
+        <f t="array" aca="1" ref="J32" ca="1">INDIRECT(ADDRESS(4+$C$32,6))</f>
+        <v>60</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2384,17 +2619,24 @@
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="G33" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="50" cm="1">
+        <f t="array" aca="1" ref="H33" ca="1">INDIRECT(ADDRESS(4+$C$32,IF($D$32=0,9,IF($D$32=1,13,17))))</f>
+        <v>115</v>
+      </c>
+      <c r="I33" s="50" cm="1">
+        <f t="array" aca="1" ref="I33" ca="1">INDIRECT(ADDRESS(4+$C$32,IF($D$32=0,10,IF($D$32=1,14,18))))</f>
+        <v>6.5</v>
+      </c>
+      <c r="J33" s="51" cm="1">
+        <f t="array" aca="1" ref="J33" ca="1">INDIRECT(ADDRESS(4+$C$32,IF($D$32=0,11,IF($D$32=1,15,19))))</f>
+        <v>47</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2424,17 +2666,9 @@
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2464,17 +2698,19 @@
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2507,14 +2743,21 @@
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="G36" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <f ca="1">IF(MOD(H33, I32) = 0, QUOTIENT(H33,I32), QUOTIENT(H33,I32)+1)</f>
+        <v>17</v>
+      </c>
+      <c r="I36" s="5">
+        <f ca="1">H36*J32</f>
+        <v>1020</v>
+      </c>
+      <c r="J36" s="26">
+        <f ca="1">IF($I$36&gt;$I$37,$H$41, $G$41)</f>
+        <v>0</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2544,17 +2787,24 @@
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="G37" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="7">
+        <f ca="1">IF(MOD(H32, I33) = 0, QUOTIENT(H32,I33), QUOTIENT(H32,I33)+1)</f>
+        <v>16</v>
+      </c>
+      <c r="I37" s="7">
+        <f ca="1">H37*J33</f>
+        <v>752</v>
+      </c>
+      <c r="J37" s="23">
+        <f ca="1">IF($I$37&gt;$I$36,$H$41, $G$41)</f>
+        <v>1</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2587,10 +2837,6 @@
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2624,16 +2870,11 @@
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2664,16 +2905,15 @@
       <c r="AK39" s="1"/>
       <c r="AL39" s="1"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="G40" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2704,16 +2944,15 @@
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="G41" s="22">
+        <v>1</v>
+      </c>
+      <c r="H41" s="23">
+        <v>0</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2747,10 +2986,6 @@
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2786,12 +3021,6 @@
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2826,12 +3055,6 @@
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2866,12 +3089,6 @@
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2906,12 +3123,6 @@
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2946,12 +3157,6 @@
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2986,12 +3191,6 @@
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -3026,12 +3225,6 @@
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -3066,12 +3259,6 @@
     </row>
     <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -3106,12 +3293,6 @@
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -3145,15 +3326,19 @@
       <c r="AL51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="N17:Q17"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>